<commit_message>
valid BST / uf ...
</commit_message>
<xml_diff>
--- a/js/leetcode/js/leetcode.xlsx
+++ b/js/leetcode/js/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/XiumingXu/Development/Kata/js/leetcode/js/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC1555D-BBD7-3246-B63F-0929921BC7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752293FD-A4B5-E942-9422-D2D206CA857F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="29300" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{D9979169-2470-B940-A4AE-C3D5CB1A8763}"/>
+    <workbookView xWindow="12920" yWindow="29300" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{D9979169-2470-B940-A4AE-C3D5CB1A8763}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="641">
   <si>
     <t>1249 Minimum Remove to Make Valid Parentheses            </t>
   </si>
@@ -1994,12 +1994,62 @@
   <si>
     <t>神奇, 就从最后一个开始往前头</t>
   </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Max 取当前的start 线性</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if 条件中的l 被减之后不会 进入其他的分支</t>
+  </si>
+  <si>
+    <t>二维数组的intialize</t>
+  </si>
+  <si>
+    <r>
+      <t>还是老实的写</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> / | 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>而不是右移把</t>
+    </r>
+  </si>
+  <si>
+    <t>有的时候 提出来的反而不咋地</t>
+  </si>
+  <si>
+    <t>滑动窗口类似于一种控制变量法, 保持一个恒定值 presum + 二分  / 滑动窗口, java有 arrays.binarySearch</t>
+  </si>
+  <si>
+    <t>双指针还是要看看</t>
+  </si>
+  <si>
+    <t>后续遍历, 跟之前的前序不太一样</t>
+  </si>
+  <si>
+    <t>是不是环 就用connect 有一个公共parent 就是环</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2176,6 +2226,11 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2299,7 +2354,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2350,12 +2405,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2364,6 +2413,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3020,7 +3076,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="40" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3031,7 +3087,7 @@
       <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="41"/>
     </row>
     <row r="30" spans="1:5" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -8372,8 +8428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD386AB-BC84-7443-A7E1-450D0CF9B325}">
   <dimension ref="A1:G317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8490,7 +8546,7 @@
       <c r="D8" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
@@ -8572,13 +8628,13 @@
       <c r="D14" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="38" t="s">
         <v>613</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="37" t="s">
         <v>611</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="37" t="s">
         <v>612</v>
       </c>
     </row>
@@ -8864,7 +8920,7 @@
       <c r="C36" s="30">
         <v>0.68700000000000006</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="39" t="s">
         <v>217</v>
       </c>
       <c r="E36" s="32" t="s">
@@ -9153,6 +9209,9 @@
       <c r="D60" s="17" t="s">
         <v>217</v>
       </c>
+      <c r="E60" s="19" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
@@ -9165,6 +9224,9 @@
       <c r="D61" s="17" t="s">
         <v>217</v>
       </c>
+      <c r="E61" s="19" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="19"/>
@@ -9177,6 +9239,9 @@
       <c r="D62" s="17" t="s">
         <v>217</v>
       </c>
+      <c r="E62" s="19" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
@@ -9189,6 +9254,9 @@
       <c r="D63" s="17" t="s">
         <v>217</v>
       </c>
+      <c r="E63" s="19" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
@@ -9201,8 +9269,11 @@
       <c r="D64" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="19" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="6" t="s">
         <v>387</v>
@@ -9213,8 +9284,9 @@
       <c r="D65" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="19"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="19"/>
       <c r="B66" s="6" t="s">
         <v>388</v>
@@ -9225,8 +9297,9 @@
       <c r="D66" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="19"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="19"/>
       <c r="B67" s="6" t="s">
         <v>390</v>
@@ -9237,8 +9310,14 @@
       <c r="D67" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="F67" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="19"/>
       <c r="B68" s="6" t="s">
         <v>391</v>
@@ -9249,8 +9328,9 @@
       <c r="D68" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="19"/>
+    </row>
+    <row r="69" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="6" t="s">
         <v>392</v>
@@ -9261,8 +9341,12 @@
       <c r="D69" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="17"/>
+      <c r="F69" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="6" t="s">
         <v>394</v>
@@ -9273,8 +9357,9 @@
       <c r="D70" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="42"/>
+    </row>
+    <row r="71" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="6" t="s">
         <v>395</v>
@@ -9285,8 +9370,9 @@
       <c r="D71" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="36"/>
+    </row>
+    <row r="72" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="19"/>
       <c r="B72" s="6" t="s">
         <v>399</v>
@@ -9297,8 +9383,9 @@
       <c r="D72" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="36"/>
+    </row>
+    <row r="73" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="6" t="s">
         <v>405</v>
@@ -9309,8 +9396,11 @@
       <c r="D73" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="42" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B74" s="6" t="s">
         <v>406</v>
       </c>
@@ -9321,7 +9411,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="s">
         <v>408</v>
       </c>
@@ -9332,7 +9422,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" s="6" t="s">
         <v>409</v>
       </c>
@@ -9343,7 +9433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" s="6" t="s">
         <v>412</v>
       </c>
@@ -9354,7 +9444,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B78" s="6" t="s">
         <v>414</v>
       </c>
@@ -9365,7 +9455,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" s="6" t="s">
         <v>419</v>
       </c>
@@ -9376,7 +9466,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" s="6" t="s">
         <v>420</v>
       </c>
@@ -10455,7 +10545,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B177" s="33" t="s">
         <v>319</v>
       </c>
@@ -10466,7 +10556,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B178" s="6" t="s">
         <v>322</v>
       </c>
@@ -10483,7 +10573,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B179" s="6" t="s">
         <v>330</v>
       </c>
@@ -10498,7 +10588,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B180" s="6" t="s">
         <v>335</v>
       </c>
@@ -10515,7 +10605,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B181" s="6" t="s">
         <v>273</v>
       </c>
@@ -10529,7 +10619,8 @@
         <v>602</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="19"/>
       <c r="B182" s="6" t="s">
         <v>342</v>
       </c>
@@ -10540,7 +10631,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="19"/>
       <c r="B183" s="6" t="s">
         <v>344</v>
       </c>
@@ -10551,7 +10643,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="19"/>
       <c r="B184" s="6" t="s">
         <v>345</v>
       </c>
@@ -10562,7 +10655,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="19"/>
       <c r="B185" s="6" t="s">
         <v>350</v>
       </c>
@@ -10573,7 +10667,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="19"/>
       <c r="B186" s="6" t="s">
         <v>351</v>
       </c>
@@ -10584,7 +10679,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="19"/>
       <c r="B187" s="6" t="s">
         <v>352</v>
       </c>
@@ -10595,7 +10691,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B188" s="6" t="s">
         <v>356</v>
       </c>
@@ -10606,7 +10702,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B189" s="29" t="s">
         <v>362</v>
       </c>
@@ -10624,7 +10720,7 @@
       </c>
       <c r="G189" s="32"/>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B190" s="6" t="s">
         <v>290</v>
       </c>
@@ -10638,7 +10734,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B191" s="6" t="s">
         <v>385</v>
       </c>
@@ -10650,7 +10746,7 @@
       </c>
       <c r="E191" s="19"/>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B192" s="6" t="s">
         <v>389</v>
       </c>
@@ -10662,7 +10758,10 @@
       </c>
       <c r="E192" s="19"/>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>631</v>
+      </c>
       <c r="B193" s="26" t="s">
         <v>396</v>
       </c>
@@ -10673,7 +10772,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B194" s="6" t="s">
         <v>403</v>
       </c>
@@ -10687,7 +10786,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B195" s="6" t="s">
         <v>404</v>
       </c>
@@ -10698,7 +10797,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B196" s="6" t="s">
         <v>413</v>
       </c>
@@ -10709,7 +10808,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B197" s="6" t="s">
         <v>421</v>
       </c>
@@ -10720,7 +10819,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B198" s="6" t="s">
         <v>432</v>
       </c>
@@ -10731,7 +10830,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B199" s="6" t="s">
         <v>436</v>
       </c>
@@ -10742,7 +10841,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B200" s="6" t="s">
         <v>437</v>
       </c>
@@ -10753,7 +10852,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B201" s="6" t="s">
         <v>438</v>
       </c>
@@ -10764,7 +10863,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B202" s="6" t="s">
         <v>441</v>
       </c>
@@ -10775,7 +10874,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B203" s="6" t="s">
         <v>446</v>
       </c>
@@ -10786,7 +10885,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B204" s="6" t="s">
         <v>455</v>
       </c>
@@ -10797,7 +10896,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B205" s="6" t="s">
         <v>468</v>
       </c>
@@ -10808,7 +10907,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B206" s="6" t="s">
         <v>470</v>
       </c>
@@ -10819,7 +10918,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B207" s="6" t="s">
         <v>483</v>
       </c>
@@ -10830,7 +10929,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B208" s="6" t="s">
         <v>492</v>
       </c>

</xml_diff>

<commit_message>
add some strang questions
</commit_message>
<xml_diff>
--- a/js/leetcode/js/leetcode.xlsx
+++ b/js/leetcode/js/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/XiumingXu/Development/Kata/js/leetcode/js/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B302BB1-A98E-DB46-AF87-E90949898D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30A9E2A-0D76-284F-8639-D9C7EC059492}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="29300" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{D9979169-2470-B940-A4AE-C3D5CB1A8763}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33280" windowHeight="20500" activeTab="4" xr2:uid="{D9979169-2470-B940-A4AE-C3D5CB1A8763}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="664">
   <si>
     <t>1249 Minimum Remove to Make Valid Parentheses            </t>
   </si>
@@ -2094,6 +2094,24 @@
   </si>
   <si>
     <t>看一下 循环还是怎样??  反转链表 并没有用dummy head</t>
+  </si>
+  <si>
+    <t>差值法 不是以 a为基点</t>
+  </si>
+  <si>
+    <t>先右后左中序遍历</t>
+  </si>
+  <si>
+    <t>二分 临界值, 每次如何以以及他, 双指针好像一点</t>
+  </si>
+  <si>
+    <t>序列化 + hashmap</t>
+  </si>
+  <si>
+    <t>很繁琐的题 分四种情况讨论</t>
+  </si>
+  <si>
+    <t>感觉没什么的 注意tail和head都要上</t>
   </si>
 </sst>
 </file>
@@ -2405,7 +2423,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2471,6 +2489,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -8479,8 +8498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD386AB-BC84-7443-A7E1-450D0CF9B325}">
   <dimension ref="A1:G317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="139" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="150" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9751,8 +9770,7 @@
       </c>
       <c r="E96" s="19"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="19"/>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
         <v>451</v>
       </c>
@@ -9763,8 +9781,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="19"/>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98" s="6" t="s">
         <v>452</v>
       </c>
@@ -9774,9 +9791,11 @@
       <c r="D98" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="19"/>
+      <c r="E98" s="19" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99" s="6" t="s">
         <v>454</v>
       </c>
@@ -9786,9 +9805,9 @@
       <c r="D99" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="19"/>
+      <c r="E99" s="19"/>
+    </row>
+    <row r="100" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="6" t="s">
         <v>456</v>
       </c>
@@ -9798,8 +9817,9 @@
       <c r="D100" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" s="19"/>
+    </row>
+    <row r="101" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="19"/>
       <c r="B101" s="6" t="s">
         <v>457</v>
@@ -9810,8 +9830,9 @@
       <c r="D101" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" s="36"/>
+    </row>
+    <row r="102" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="19"/>
       <c r="B102" s="6" t="s">
         <v>458</v>
@@ -9822,8 +9843,9 @@
       <c r="D102" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" s="36"/>
+    </row>
+    <row r="103" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="19"/>
       <c r="B103" s="6" t="s">
         <v>460</v>
@@ -9834,9 +9856,11 @@
       <c r="D103" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="19"/>
+      <c r="E103" s="36" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>462</v>
       </c>
@@ -9846,8 +9870,9 @@
       <c r="D104" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" s="40"/>
+    </row>
+    <row r="105" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="19"/>
       <c r="B105" s="6" t="s">
         <v>463</v>
@@ -9858,9 +9883,11 @@
       <c r="D105" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="19"/>
+      <c r="E105" s="36" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
         <v>464</v>
       </c>
@@ -9870,8 +9897,11 @@
       <c r="D106" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" s="19" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="19"/>
       <c r="B107" s="6" t="s">
         <v>465</v>
@@ -9882,8 +9912,11 @@
       <c r="D107" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" s="36" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="19"/>
       <c r="B108" s="6" t="s">
         <v>466</v>
@@ -9894,8 +9927,9 @@
       <c r="D108" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" s="40"/>
+    </row>
+    <row r="109" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="19"/>
       <c r="B109" s="6" t="s">
         <v>467</v>
@@ -9906,8 +9940,10 @@
       <c r="D109" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" s="36"/>
+    </row>
+    <row r="110" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="19"/>
       <c r="B110" s="6" t="s">
         <v>469</v>
       </c>
@@ -9917,8 +9953,12 @@
       <c r="D110" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" s="19" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="19"/>
       <c r="B111" s="6" t="s">
         <v>471</v>
       </c>
@@ -9928,8 +9968,12 @@
       <c r="D111" s="17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111" s="43" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="19"/>
       <c r="B112" s="6" t="s">
         <v>472</v>
       </c>
@@ -9940,7 +9984,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="19"/>
       <c r="B113" s="6" t="s">
         <v>475</v>
       </c>
@@ -9951,7 +9996,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="19"/>
       <c r="B114" s="6" t="s">
         <v>477</v>
       </c>
@@ -9962,7 +10008,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="19"/>
       <c r="B115" s="6" t="s">
         <v>478</v>
       </c>
@@ -9973,7 +10020,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="19"/>
       <c r="B116" s="6" t="s">
         <v>479</v>
       </c>
@@ -9984,7 +10032,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="19"/>
       <c r="B117" s="6" t="s">
         <v>480</v>
       </c>
@@ -9995,7 +10044,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="19"/>
       <c r="B118" s="6" t="s">
         <v>484</v>
       </c>
@@ -10006,7 +10056,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="19"/>
       <c r="B119" s="6" t="s">
         <v>485</v>
       </c>
@@ -10017,7 +10068,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="19"/>
       <c r="B120" s="26" t="s">
         <v>486</v>
       </c>
@@ -10028,7 +10080,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="19"/>
       <c r="B121" s="6" t="s">
         <v>487</v>
       </c>
@@ -10039,7 +10092,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="19"/>
       <c r="B122" s="6" t="s">
         <v>488</v>
       </c>
@@ -10050,7 +10104,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="19"/>
       <c r="B123" s="6" t="s">
         <v>490</v>
       </c>
@@ -10061,7 +10116,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="19"/>
       <c r="B124" s="6" t="s">
         <v>491</v>
       </c>
@@ -10072,7 +10128,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B125" s="6" t="s">
         <v>493</v>
       </c>
@@ -10083,7 +10139,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B126" s="6" t="s">
         <v>496</v>
       </c>
@@ -10094,7 +10150,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B127" s="6" t="s">
         <v>497</v>
       </c>
@@ -10105,7 +10161,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B128" s="6" t="s">
         <v>498</v>
       </c>
@@ -10610,6 +10666,7 @@
       <c r="D173" s="28" t="s">
         <v>215</v>
       </c>
+      <c r="E173" s="19"/>
     </row>
     <row r="174" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B174" s="6" t="s">

</xml_diff>